<commit_message>
Election.Analytic.System - PPRP  #328 - Update Excel files.
</commit_message>
<xml_diff>
--- a/Imports/Excels/รายชื่อว่าที่ผู้สมัครปี 2566 v3.7.xlsx
+++ b/Imports/Excels/รายชื่อว่าที่ผู้สมัครปี 2566 v3.7.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="324">
   <si>
     <t>จังหวัด</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>กลุ่มย่อย</t>
+  </si>
+  <si>
+    <t>ข้อมูลทดสอบ หมายเหตุ</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1610,7 +1613,7 @@
     <col min="5" max="5" width="39.5546875" style="24" customWidth="1"/>
     <col min="6" max="6" width="43.5546875" style="24" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.21875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1660,7 +1663,9 @@
       <c r="G2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="42" customHeight="1">
       <c r="A3" s="12" t="s">

</xml_diff>